<commit_message>
sistemati algoritmi e log
per dividi_cerca ora l'unione viene fatta solo nella cartella dei trovati, mentre nel comverter non è cambiato quasi nulla
</commit_message>
<xml_diff>
--- a/Dividi_Cerca_PdfCF/CF.xlsx
+++ b/Dividi_Cerca_PdfCF/CF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Haider Maqsood\Documents\GitHub\MAW\Dividi_Cerca_PdfCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5265BFF2-9575-4417-9965-355904537FFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF727DC9-E86A-44CB-9C7F-72142A7085AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>cercare</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>BDLBSM93H46Z336M</t>
+  </si>
+  <si>
+    <t>BBSMHR90T17Z236E</t>
+  </si>
+  <si>
+    <t>BSADVD95H21D612A</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +559,21 @@
         <v>18</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>